<commit_message>
Made changes in relation creation
</commit_message>
<xml_diff>
--- a/Entity Linking/Mapping/new_mapping_master.xlsx
+++ b/Entity Linking/Mapping/new_mapping_master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uscedu-my.sharepoint.com/personal/ondanatv_usc_edu/Documents/USC Classes/558/Project/Work/fitness_kg/Entity Linking/Mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="8_{B4E704BE-A85D-41EA-A125-ABE4957BC88F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E553A39-25A1-441C-9460-3C75827D5713}"/>
+  <xr:revisionPtr revIDLastSave="162" documentId="8_{B4E704BE-A85D-41EA-A125-ABE4957BC88F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E93A3D6-B95F-4141-AC32-A61267603101}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{FF8D9DF3-E641-4141-89AA-2E6C1E93F692}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FF8D9DF3-E641-4141-89AA-2E6C1E93F692}"/>
   </bookViews>
   <sheets>
     <sheet name="Yoga Name Mapping" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="317">
   <si>
     <t>AlternateName</t>
   </si>
@@ -955,13 +955,55 @@
   </si>
   <si>
     <t>anatomy</t>
+  </si>
+  <si>
+    <t>sirsasana</t>
+  </si>
+  <si>
+    <t>bharadvajasana</t>
+  </si>
+  <si>
+    <t>wide-legged forward bend pose</t>
+  </si>
+  <si>
+    <t>supta padangustasana</t>
+  </si>
+  <si>
+    <t>chaturanga</t>
+  </si>
+  <si>
+    <t>setu bandha</t>
+  </si>
+  <si>
+    <t>warrior i</t>
+  </si>
+  <si>
+    <t>downward-facing dog pose.</t>
+  </si>
+  <si>
+    <t>warrior pose i</t>
+  </si>
+  <si>
+    <t>reclining hand-to-big toe pose i</t>
+  </si>
+  <si>
+    <t>marichi's pose,</t>
+  </si>
+  <si>
+    <t>warrior ii</t>
+  </si>
+  <si>
+    <t>reverse plank pose</t>
+  </si>
+  <si>
+    <t>pashchimottanasana</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -976,6 +1018,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1028,7 +1076,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1037,6 +1085,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1412,10 +1463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A533809E-1161-463A-952D-DF2E7A62718E}">
-  <dimension ref="A1:B119"/>
+  <dimension ref="A1:C133"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1434,7 +1485,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>304</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -1442,127 +1493,127 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>308</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
         <v>31</v>
@@ -1570,824 +1621,938 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>310</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B34" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B36" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B37" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B38" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>71</v>
+        <v>307</v>
       </c>
       <c r="B39" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B40" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B41" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B42" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B43" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B44" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B45" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B46" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B47" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B48" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B49" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B50" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B51" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B52" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B53" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B54" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B55" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B56" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B57" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B58" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B59" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B60" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B61" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B62" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B63" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B64" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B65" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>123</v>
+        <v>313</v>
       </c>
       <c r="B66" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B67" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B68" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B69" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B70" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>132</v>
+        <v>312</v>
       </c>
       <c r="B71" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>134</v>
+        <v>306</v>
       </c>
       <c r="B72" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="B73" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="B74" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>140</v>
+        <v>315</v>
       </c>
       <c r="B75" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="B76" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="B77" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="B78" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="B79" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
+        <v>134</v>
+      </c>
+      <c r="B80" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>136</v>
+      </c>
+      <c r="B81" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>138</v>
+      </c>
+      <c r="B82" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>140</v>
+      </c>
+      <c r="B83" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>316</v>
+      </c>
+      <c r="B84" t="s">
+        <v>141</v>
+      </c>
+      <c r="C84" s="8"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>142</v>
+      </c>
+      <c r="B85" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>144</v>
+      </c>
+      <c r="B86" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>146</v>
+      </c>
+      <c r="B87" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>147</v>
+      </c>
+      <c r="B88" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
         <v>148</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B89" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
         <v>150</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B90" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
         <v>152</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B91" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
         <v>153</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B92" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
         <v>155</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B93" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
         <v>157</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B94" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
         <v>159</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B95" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>161</v>
-      </c>
-      <c r="B87" t="s">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>303</v>
+      </c>
+      <c r="B96" t="s">
         <v>162</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>163</v>
-      </c>
-      <c r="B88" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>165</v>
-      </c>
-      <c r="B89" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>167</v>
-      </c>
-      <c r="B90" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>169</v>
-      </c>
-      <c r="B91" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>171</v>
-      </c>
-      <c r="B92" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>173</v>
-      </c>
-      <c r="B93" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>175</v>
-      </c>
-      <c r="B94" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>176</v>
-      </c>
-      <c r="B95" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
-        <v>178</v>
-      </c>
-      <c r="B96" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="B97" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
       <c r="B98" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="B99" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="B100" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="B101" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="B102" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>187</v>
+        <v>309</v>
       </c>
       <c r="B103" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="B104" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="B105" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
       <c r="B106" t="s">
-        <v>31</v>
+        <v>177</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="B107" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
       <c r="B108" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="B109" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="B110" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
       <c r="B111" t="s">
-        <v>202</v>
+        <v>183</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>203</v>
+        <v>185</v>
       </c>
       <c r="B112" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
       <c r="B113" t="s">
-        <v>124</v>
+        <v>183</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
       <c r="B114" t="s">
-        <v>68</v>
+        <v>209</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
+        <v>189</v>
+      </c>
+      <c r="B115" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>191</v>
+      </c>
+      <c r="B116" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>193</v>
+      </c>
+      <c r="B117" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>194</v>
+      </c>
+      <c r="B118" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>196</v>
+      </c>
+      <c r="B119" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>198</v>
+      </c>
+      <c r="B120" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>199</v>
+      </c>
+      <c r="B121" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>201</v>
+      </c>
+      <c r="B122" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>203</v>
+      </c>
+      <c r="B123" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>205</v>
+      </c>
+      <c r="B124" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>206</v>
+      </c>
+      <c r="B125" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
         <v>207</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B126" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A116" s="2" t="s">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B127" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A117" s="2" t="s">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B128" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A118" s="2" t="s">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B129" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A119" s="2" t="s">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B130" t="s">
         <v>190</v>
       </c>
     </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>305</v>
+      </c>
+      <c r="B131" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>311</v>
+      </c>
+      <c r="B132" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>314</v>
+      </c>
+      <c r="B133" t="s">
+        <v>177</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A18">
+  <conditionalFormatting sqref="A20">
     <cfRule type="duplicateValues" dxfId="5" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B18">
+  <conditionalFormatting sqref="B20">
     <cfRule type="duplicateValues" dxfId="4" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A114:A119 A1:A112 B113">
+  <conditionalFormatting sqref="A125:A130 A1:A71 B124 A73:A83 A85:A123">
     <cfRule type="duplicateValues" dxfId="3" priority="1"/>
     <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2546,7 +2711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8251FA6-454B-414F-AAB8-EAD6CF4C9964}">
   <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+    <sheetView topLeftCell="A48" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>

</xml_diff>